<commit_message>
Find first unique char
</commit_message>
<xml_diff>
--- a/DSA(2024).xlsx
+++ b/DSA(2024).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaMasterClass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA5FAA97-62A1-4D94-A653-66E8B442E55F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E673C6-9065-4319-9853-3E8D159AA156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="80">
   <si>
     <t>01-01-2024</t>
   </si>
@@ -262,6 +262,9 @@
   </si>
   <si>
     <t>PRACTICE(*)</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -350,14 +353,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -389,6 +384,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -778,43 +781,43 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="70.5546875" style="11" customWidth="1"/>
-    <col min="3" max="3" width="19" style="19" customWidth="1"/>
+    <col min="2" max="2" width="70.5546875" customWidth="1"/>
+    <col min="3" max="3" width="19" style="15" customWidth="1"/>
     <col min="4" max="4" width="18.109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="103.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="17" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:8" s="13" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="12" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="22" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="19">
+      <c r="C2" s="15">
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -826,11 +829,11 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="15">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -844,10 +847,10 @@
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="20"/>
+      <c r="C4" s="16"/>
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
@@ -862,7 +865,7 @@
       <c r="B5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="15">
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -879,10 +882,13 @@
       <c r="B6" s="7" t="s">
         <v>14</v>
       </c>
+      <c r="C6" s="15">
+        <v>1</v>
+      </c>
       <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="23" t="s">
         <v>15</v>
       </c>
     </row>
@@ -890,10 +896,12 @@
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="21"/>
+      <c r="C7" s="17" t="s">
+        <v>79</v>
+      </c>
       <c r="D7" s="1" t="s">
         <v>8</v>
       </c>
@@ -916,10 +924,10 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -930,8 +938,8 @@
       </c>
     </row>
     <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9"/>
-      <c r="B10" s="11" t="s">
+      <c r="A10" s="22"/>
+      <c r="B10" t="s">
         <v>25</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -943,7 +951,7 @@
       <c r="A11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -957,7 +965,7 @@
       <c r="A12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" t="s">
         <v>30</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -974,7 +982,7 @@
       <c r="B13" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="20"/>
+      <c r="C13" s="16"/>
       <c r="D13" s="1" t="s">
         <v>2</v>
       </c>
@@ -986,7 +994,7 @@
       <c r="A14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" t="s">
         <v>36</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1000,7 +1008,7 @@
       <c r="A15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" t="s">
         <v>39</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1014,7 +1022,7 @@
       <c r="A16" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" t="s">
         <v>42</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1028,7 +1036,7 @@
       <c r="A17" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" t="s">
         <v>45</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -1042,7 +1050,7 @@
       <c r="A18" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" t="s">
         <v>49</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -1054,7 +1062,7 @@
       <c r="A19" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" t="s">
         <v>51</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -1068,10 +1076,10 @@
       <c r="A20" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="19">
+      <c r="C20" s="15">
         <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -1085,10 +1093,10 @@
       <c r="A21" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="19">
+      <c r="C21" s="15">
         <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -1099,13 +1107,13 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="21" t="s">
         <v>8</v>
       </c>
       <c r="E22" s="4" t="s">
@@ -1113,9 +1121,9 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="36.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="10"/>
-      <c r="B23" s="12"/>
-      <c r="D23" s="10"/>
+      <c r="A23" s="21"/>
+      <c r="B23" s="20"/>
+      <c r="D23" s="21"/>
       <c r="E23" s="4" t="s">
         <v>61</v>
       </c>
@@ -1124,10 +1132,10 @@
       <c r="A24" s="2">
         <v>45424</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="19">
+      <c r="C24" s="15">
         <v>1</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -1144,7 +1152,7 @@
       <c r="B25" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C25" s="22">
+      <c r="C25" s="18">
         <v>1</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -1158,7 +1166,7 @@
       <c r="A26" s="2">
         <v>45427</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" t="s">
         <v>68</v>
       </c>
       <c r="D26" s="1" t="s">
@@ -1175,7 +1183,7 @@
       <c r="B27" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="20"/>
+      <c r="C27" s="16"/>
       <c r="D27" s="1" t="s">
         <v>8</v>
       </c>
@@ -1185,10 +1193,10 @@
       <c r="A28" s="2">
         <v>45569</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B28" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="19">
+      <c r="C28" s="15">
         <v>1</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -1202,10 +1210,10 @@
       <c r="A29" s="2">
         <v>45588</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="19">
+      <c r="C29" s="15">
         <v>1</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1217,10 +1225,10 @@
       <c r="A30" s="2">
         <v>45607</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B30" t="s">
         <v>73</v>
       </c>
-      <c r="C30" s="19">
+      <c r="C30" s="15">
         <v>1</v>
       </c>
       <c r="D30" s="1" t="s">

</xml_diff>

<commit_message>
Smallest letter greater than target
</commit_message>
<xml_diff>
--- a/DSA(2024).xlsx
+++ b/DSA(2024).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaMasterClass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E673C6-9065-4319-9853-3E8D159AA156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A846CF9-3518-48C5-9C18-3B8A8E80334C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="76">
   <si>
     <t>01-01-2024</t>
   </si>
@@ -75,15 +75,6 @@
     <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/127/strings/881/</t>
   </si>
   <si>
-    <t>05-01-2024</t>
-  </si>
-  <si>
-    <t>Remove Duplicates from Sorted Array</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/explore/featured/card/top-interview-questions-easy/92/array/727/</t>
-  </si>
-  <si>
     <t>06-01-2024</t>
   </si>
   <si>
@@ -262,9 +253,6 @@
   </si>
   <si>
     <t>PRACTICE(*)</t>
-  </si>
-  <si>
-    <t>s</t>
   </si>
 </sst>
 </file>
@@ -329,7 +317,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -356,9 +344,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -376,14 +361,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -391,7 +374,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -778,46 +760,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="70.5546875" customWidth="1"/>
-    <col min="3" max="3" width="19" style="15" customWidth="1"/>
+    <col min="3" max="3" width="19" style="14" customWidth="1"/>
     <col min="4" max="4" width="18.109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="103.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="13" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:8" s="12" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="2" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="14">
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -829,11 +811,11 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="22"/>
+      <c r="A3" s="21"/>
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="14">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -850,7 +832,7 @@
       <c r="B4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="16"/>
+      <c r="C4" s="15"/>
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
@@ -865,7 +847,7 @@
       <c r="B5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="14">
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -882,25 +864,25 @@
       <c r="B6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="14">
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="17" t="s">
-        <v>79</v>
+      <c r="C7" s="14">
+        <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>8</v>
@@ -910,11 +892,14 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" t="s">
         <v>20</v>
+      </c>
+      <c r="C8" s="14">
+        <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>8</v>
@@ -923,31 +908,34 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="22" t="s">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="21"/>
+      <c r="B9" t="s">
         <v>22</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="B10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="22"/>
-      <c r="B10" t="s">
+      <c r="C10" s="14">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:8" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>26</v>
       </c>
@@ -961,28 +949,28 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>30</v>
       </c>
+      <c r="C12" s="15"/>
       <c r="D12" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="16"/>
       <c r="D13" s="1" t="s">
         <v>2</v>
       </c>
@@ -990,7 +978,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>35</v>
       </c>
@@ -1004,7 +992,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>38</v>
       </c>
@@ -1012,13 +1000,13 @@
         <v>39</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>41</v>
       </c>
@@ -1026,60 +1014,63 @@
         <v>42</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="B18" t="s">
         <v>48</v>
       </c>
-      <c r="B18" t="s">
+      <c r="D18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:5" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+    </row>
+    <row r="19" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B19" t="s">
         <v>51</v>
       </c>
+      <c r="C19" s="14">
+        <v>1</v>
+      </c>
       <c r="D19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B20" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C20" s="14">
         <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -1089,71 +1080,68 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:5" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="15">
-        <v>1</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="4" t="s">
+    </row>
+    <row r="22" spans="1:5" ht="36.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="20"/>
+      <c r="B22" s="19"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="21" t="s">
+    <row r="23" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>45424</v>
+      </c>
+      <c r="B23" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="C23" s="14">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>45425</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="16">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>45427</v>
+      </c>
+      <c r="B25" t="s">
         <v>65</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="36.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="21"/>
-      <c r="B23" s="20"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
-        <v>45424</v>
-      </c>
-      <c r="B24" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" s="15">
-        <v>1</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
-        <v>45425</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" s="18">
-        <v>1</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>8</v>
@@ -1162,87 +1150,73 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
-        <v>45427</v>
-      </c>
-      <c r="B26" t="s">
+        <v>45568</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="15"/>
+      <c r="D26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>45569</v>
+      </c>
+      <c r="B27" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="14">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="2">
-        <v>45568</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
-        <v>45569</v>
+        <v>45588</v>
       </c>
       <c r="B28" t="s">
-        <v>70</v>
-      </c>
-      <c r="C28" s="15">
+        <v>69</v>
+      </c>
+      <c r="C28" s="14">
         <v>1</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="6" t="s">
-        <v>71</v>
-      </c>
+      <c r="E28" s="4"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
-        <v>45588</v>
+        <v>45607</v>
       </c>
       <c r="B29" t="s">
-        <v>72</v>
-      </c>
-      <c r="C29" s="15">
+        <v>70</v>
+      </c>
+      <c r="C29" s="14">
         <v>1</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E29" s="4"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="2">
-        <v>45607</v>
-      </c>
-      <c r="B30" t="s">
-        <v>73</v>
-      </c>
-      <c r="C30" s="15">
-        <v>1</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="D21:D22"/>
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A21:A22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -1250,25 +1224,24 @@
     <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="E5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="E6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="E7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="E8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="E9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="E12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="E13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="E15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="E16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="E17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E19" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="E20" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="E21" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="E22" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="E23" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="E24" r:id="rId21" xr:uid="{C5CAB132-7B8A-4868-9CE2-EB6967D9E2C5}"/>
-    <hyperlink ref="E25" r:id="rId22" xr:uid="{60C1110F-5F35-4BA3-BE0E-5D2B2A5A0CB4}"/>
-    <hyperlink ref="E26" r:id="rId23" xr:uid="{CF0FEC0D-8FF8-4FA8-9FED-790E8E16F911}"/>
-    <hyperlink ref="E28" r:id="rId24" xr:uid="{9DAD39F5-2A80-4390-9BA5-B159E91EB2B4}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="E15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="E16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E18" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E19" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="E20" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="E21" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="E22" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="E23" r:id="rId20" xr:uid="{C5CAB132-7B8A-4868-9CE2-EB6967D9E2C5}"/>
+    <hyperlink ref="E24" r:id="rId21" xr:uid="{60C1110F-5F35-4BA3-BE0E-5D2B2A5A0CB4}"/>
+    <hyperlink ref="E25" r:id="rId22" xr:uid="{CF0FEC0D-8FF8-4FA8-9FED-790E8E16F911}"/>
+    <hyperlink ref="E27" r:id="rId23" xr:uid="{9DAD39F5-2A80-4390-9BA5-B159E91EB2B4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Search in montain array
</commit_message>
<xml_diff>
--- a/DSA(2024).xlsx
+++ b/DSA(2024).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaMasterClass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A846CF9-3518-48C5-9C18-3B8A8E80334C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F60336-D489-44A9-862E-9EC01A543937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -763,7 +763,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -942,6 +942,9 @@
       <c r="B11" t="s">
         <v>27</v>
       </c>
+      <c r="C11" s="14">
+        <v>1</v>
+      </c>
       <c r="D11" s="1" t="s">
         <v>8</v>
       </c>
@@ -956,7 +959,9 @@
       <c r="B12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="15"/>
+      <c r="C12" s="15">
+        <v>1</v>
+      </c>
       <c r="D12" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Convert string to integer
</commit_message>
<xml_diff>
--- a/DSA(2024).xlsx
+++ b/DSA(2024).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaMasterClass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6D7CF4-DDD5-4E3D-8BBC-412AEC468FAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF8E398A-303A-4734-BC3B-23E50D3F1A97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="74">
   <si>
     <t>01-01-2024</t>
   </si>
@@ -150,18 +150,6 @@
     <t>https://www.geeksforgeeks.org/find-rotation-count-rotated-sorted-array/</t>
   </si>
   <si>
-    <t>16-01-2024</t>
-  </si>
-  <si>
-    <t>Split Array Largest Sum</t>
-  </si>
-  <si>
-    <t>Hard</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/split-array-largest-sum/</t>
-  </si>
-  <si>
     <t>17-01-2024</t>
   </si>
   <si>
@@ -253,6 +241,12 @@
   </si>
   <si>
     <t>PRACTICE(*)</t>
+  </si>
+  <si>
+    <t>Convert String to an Integer (myAtoi)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/string-to-integer-atoi/</t>
   </si>
 </sst>
 </file>
@@ -763,7 +757,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -777,19 +771,19 @@
   <sheetData>
     <row r="1" spans="1:8" s="12" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>75</v>
-      </c>
       <c r="D1" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1014,7 +1008,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>41</v>
       </c>
@@ -1022,164 +1016,167 @@
         <v>42</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="B17" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="D17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B17" t="s">
+    </row>
+    <row r="18" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:5" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="B18" t="s">
         <v>47</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" s="14">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="3" t="s">
+    </row>
+    <row r="19" spans="1:5" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="B19" t="s">
         <v>50</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" s="14">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="14">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="4" t="s">
+    </row>
+    <row r="20" spans="1:5" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="20" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="B20" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="14">
+        <v>1</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B20" t="s">
+    </row>
+    <row r="21" spans="1:5" ht="36.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="20"/>
+      <c r="B21" s="19"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="14">
-        <v>1</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="4" t="s">
+    </row>
+    <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>45424</v>
+      </c>
+      <c r="B22" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="20" t="s">
+      <c r="C22" s="14">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="19" t="s">
+    </row>
+    <row r="23" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>45425</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="16">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>45427</v>
+      </c>
+      <c r="B24" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>45568</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="14">
-        <v>1</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="36.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="20"/>
-      <c r="B22" s="19"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
-        <v>45424</v>
-      </c>
-      <c r="B23" t="s">
-        <v>59</v>
-      </c>
-      <c r="C23" s="14">
-        <v>1</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
-        <v>45425</v>
-      </c>
-      <c r="B24" s="8" t="s">
+      <c r="C25" s="15"/>
+      <c r="D25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>45569</v>
+      </c>
+      <c r="B26" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="16">
-        <v>1</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
-        <v>45427</v>
-      </c>
-      <c r="B25" t="s">
-        <v>65</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="5" t="s">
+      <c r="C26" s="14">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="6" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
-        <v>45568</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" s="15"/>
-      <c r="D26" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
-        <v>45569</v>
+        <v>45588</v>
       </c>
       <c r="B27" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C27" s="14">
         <v>1</v>
@@ -1187,16 +1184,14 @@
       <c r="D27" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="6" t="s">
-        <v>68</v>
-      </c>
+      <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
-        <v>45588</v>
+        <v>45607</v>
       </c>
       <c r="B28" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C28" s="14">
         <v>1</v>
@@ -1208,10 +1203,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
-        <v>45607</v>
+        <v>45788</v>
       </c>
       <c r="B29" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C29" s="14">
         <v>1</v>
@@ -1219,15 +1214,17 @@
       <c r="D29" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="4"/>
+      <c r="E29" s="6" t="s">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="D20:D21"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A20:A21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -1243,16 +1240,16 @@
     <hyperlink ref="E13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="E14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
     <hyperlink ref="E15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="E16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E18" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="E19" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="E20" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="E21" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="E22" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="E23" r:id="rId20" xr:uid="{C5CAB132-7B8A-4868-9CE2-EB6967D9E2C5}"/>
-    <hyperlink ref="E24" r:id="rId21" xr:uid="{60C1110F-5F35-4BA3-BE0E-5D2B2A5A0CB4}"/>
-    <hyperlink ref="E25" r:id="rId22" xr:uid="{CF0FEC0D-8FF8-4FA8-9FED-790E8E16F911}"/>
-    <hyperlink ref="E27" r:id="rId23" xr:uid="{9DAD39F5-2A80-4390-9BA5-B159E91EB2B4}"/>
+    <hyperlink ref="E17" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E18" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="E19" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="E20" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="E21" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="E22" r:id="rId19" xr:uid="{C5CAB132-7B8A-4868-9CE2-EB6967D9E2C5}"/>
+    <hyperlink ref="E23" r:id="rId20" xr:uid="{60C1110F-5F35-4BA3-BE0E-5D2B2A5A0CB4}"/>
+    <hyperlink ref="E24" r:id="rId21" xr:uid="{CF0FEC0D-8FF8-4FA8-9FED-790E8E16F911}"/>
+    <hyperlink ref="E26" r:id="rId22" xr:uid="{9DAD39F5-2A80-4390-9BA5-B159E91EB2B4}"/>
+    <hyperlink ref="E29" r:id="rId23" xr:uid="{6609612F-5719-43A8-AFA3-447F2B3A4DE5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Length of last word
</commit_message>
<xml_diff>
--- a/DSA(2024).xlsx
+++ b/DSA(2024).xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaMasterClass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32659BB4-F310-4949-A354-FA9F590768D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3330C512-390E-4E02-806A-321695EB6CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="72">
   <si>
     <t>01-01-2024</t>
   </si>
@@ -238,13 +240,16 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/string-to-integer-atoi/</t>
+  </si>
+  <si>
+    <t>🧱 Level 1: Basics &amp; Foundations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -274,8 +279,22 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -285,6 +304,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF3B8A1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -302,7 +333,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -352,12 +383,35 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -747,8 +801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -778,15 +832,12 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="14">
-        <v>1</v>
-      </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
@@ -796,12 +847,9 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21"/>
+      <c r="A3" s="28"/>
       <c r="B3" s="7" t="s">
         <v>4</v>
-      </c>
-      <c r="C3" s="14">
-        <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
@@ -832,9 +880,6 @@
       <c r="B5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="14">
-        <v>1</v>
-      </c>
       <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
@@ -849,9 +894,6 @@
       <c r="B6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="14">
-        <v>1</v>
-      </c>
       <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
@@ -859,33 +901,28 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:8" s="24" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="14">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="C7" s="22"/>
+      <c r="D7" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="18" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="28" t="s">
         <v>19</v>
       </c>
       <c r="B8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="14">
-        <v>1</v>
-      </c>
       <c r="D8" s="1" t="s">
         <v>8</v>
       </c>
@@ -894,7 +931,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="21"/>
+      <c r="A9" s="28"/>
       <c r="B9" t="s">
         <v>22</v>
       </c>
@@ -910,9 +947,6 @@
       <c r="B10" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="14">
-        <v>1</v>
-      </c>
       <c r="D10" s="1" t="s">
         <v>8</v>
       </c>
@@ -927,9 +961,6 @@
       <c r="B11" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="14">
-        <v>1</v>
-      </c>
       <c r="D11" s="1" t="s">
         <v>8</v>
       </c>
@@ -944,9 +975,7 @@
       <c r="B12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="15">
-        <v>1</v>
-      </c>
+      <c r="C12" s="15"/>
       <c r="D12" s="1" t="s">
         <v>2</v>
       </c>
@@ -961,9 +990,6 @@
       <c r="B13" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="14">
-        <v>1</v>
-      </c>
       <c r="D13" s="1" t="s">
         <v>2</v>
       </c>
@@ -978,9 +1004,6 @@
       <c r="B14" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="14">
-        <v>1</v>
-      </c>
       <c r="D14" s="1" t="s">
         <v>2</v>
       </c>
@@ -995,9 +1018,6 @@
       <c r="B15" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="14">
-        <v>1</v>
-      </c>
       <c r="D15" s="1" t="s">
         <v>8</v>
       </c>
@@ -1005,15 +1025,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B16" t="s">
         <v>42</v>
-      </c>
-      <c r="C16" s="14">
-        <v>1</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>8</v>
@@ -1027,9 +1044,6 @@
       <c r="B17" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="14">
-        <v>1</v>
-      </c>
       <c r="D17" s="1" t="s">
         <v>8</v>
       </c>
@@ -1044,9 +1058,6 @@
       <c r="B18" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="14">
-        <v>1</v>
-      </c>
       <c r="D18" s="1" t="s">
         <v>8</v>
       </c>
@@ -1055,16 +1066,13 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="14">
-        <v>1</v>
-      </c>
-      <c r="D19" s="20" t="s">
+      <c r="D19" s="27" t="s">
         <v>8</v>
       </c>
       <c r="E19" s="4" t="s">
@@ -1072,9 +1080,9 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="36.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="20"/>
-      <c r="B20" s="19"/>
-      <c r="D20" s="20"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="26"/>
+      <c r="D20" s="27"/>
       <c r="E20" s="4" t="s">
         <v>51</v>
       </c>
@@ -1086,9 +1094,6 @@
       <c r="B21" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="14">
-        <v>1</v>
-      </c>
       <c r="D21" s="1" t="s">
         <v>8</v>
       </c>
@@ -1103,9 +1108,7 @@
       <c r="B22" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="16">
-        <v>1</v>
-      </c>
+      <c r="C22" s="16"/>
       <c r="D22" s="1" t="s">
         <v>8</v>
       </c>
@@ -1147,9 +1150,6 @@
       <c r="B25" t="s">
         <v>60</v>
       </c>
-      <c r="C25" s="14">
-        <v>1</v>
-      </c>
       <c r="D25" s="1" t="s">
         <v>8</v>
       </c>
@@ -1164,9 +1164,6 @@
       <c r="B26" t="s">
         <v>62</v>
       </c>
-      <c r="C26" s="14">
-        <v>1</v>
-      </c>
       <c r="D26" s="1" t="s">
         <v>8</v>
       </c>
@@ -1179,9 +1176,6 @@
       <c r="B27" t="s">
         <v>63</v>
       </c>
-      <c r="C27" s="14">
-        <v>1</v>
-      </c>
       <c r="D27" s="1" t="s">
         <v>8</v>
       </c>
@@ -1193,9 +1187,6 @@
       </c>
       <c r="B28" t="s">
         <v>69</v>
-      </c>
-      <c r="C28" s="14">
-        <v>1</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>8</v>
@@ -1239,4 +1230,76 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAEC6806-FDB1-4EFE-A78B-6EB62B7514F6}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="64.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" customWidth="1"/>
+    <col min="5" max="5" width="71.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="12" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="30"/>
+    </row>
+    <row r="5" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="19">
+        <v>45809</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C13" s="25"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C3:D3"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E5" r:id="rId1" xr:uid="{C7EF376E-3702-4808-933E-669DEA923A87}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Largest and second largest element
</commit_message>
<xml_diff>
--- a/DSA(2024).xlsx
+++ b/DSA(2024).xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaMasterClass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3330C512-390E-4E02-806A-321695EB6CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98EAD806-7BA7-47C6-AACC-2C6D1908B413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="74">
   <si>
     <t>01-01-2024</t>
   </si>
@@ -243,6 +242,12 @@
   </si>
   <si>
     <t>🧱 Level 1: Basics &amp; Foundations</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/problems/largest-element-in-array4009/1</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/problems/second-largest3735/1</t>
   </si>
 </sst>
 </file>
@@ -333,7 +338,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -400,10 +405,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -412,6 +413,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -801,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -832,7 +841,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="26" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -847,7 +856,7 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="28"/>
+      <c r="A3" s="26"/>
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
@@ -912,12 +921,12 @@
       <c r="D7" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="30" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="26" t="s">
         <v>19</v>
       </c>
       <c r="B8" t="s">
@@ -931,7 +940,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="28"/>
+      <c r="A9" s="26"/>
       <c r="B9" t="s">
         <v>22</v>
       </c>
@@ -1051,38 +1060,40 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:5" s="24" customFormat="1" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="4" t="s">
+      <c r="C18" s="22"/>
+      <c r="D18" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="29" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="27" t="s">
+    <row r="19" spans="1:5" s="24" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="4" t="s">
+      <c r="C19" s="22"/>
+      <c r="D19" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="29" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="36.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="27"/>
-      <c r="B20" s="26"/>
-      <c r="D20" s="27"/>
+      <c r="A20" s="32"/>
+      <c r="B20" s="31"/>
+      <c r="D20" s="32"/>
       <c r="E20" s="4" t="s">
         <v>51</v>
       </c>
@@ -1236,8 +1247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAEC6806-FDB1-4EFE-A78B-6EB62B7514F6}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1267,10 +1278,10 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="30"/>
+      <c r="D3" s="28"/>
     </row>
     <row r="5" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19">
@@ -1287,6 +1298,40 @@
       </c>
       <c r="E5" s="6" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="19">
+        <v>45809</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="19">
+        <v>45809</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1298,8 +1343,10 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E5" r:id="rId1" xr:uid="{C7EF376E-3702-4808-933E-669DEA923A87}"/>
+    <hyperlink ref="E6" r:id="rId2" xr:uid="{37D656AF-15C2-4519-B109-B0F60B16F87F}"/>
+    <hyperlink ref="E7" r:id="rId3" xr:uid="{C176BE23-95CB-44A1-B207-E06026DD7732}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Check array is sorted?
</commit_message>
<xml_diff>
--- a/DSA(2024).xlsx
+++ b/DSA(2024).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaMasterClass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98EAD806-7BA7-47C6-AACC-2C6D1908B413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE254CBB-F075-41A5-9716-A39AAE32D546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="76">
   <si>
     <t>01-01-2024</t>
   </si>
@@ -184,9 +184,6 @@
     <t>https://www.geeksforgeeks.org/problems/find-the-smallest-and-second-smallest-element-in-an-array3226/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article</t>
   </si>
   <si>
-    <t>Check if ab array sorted or not.</t>
-  </si>
-  <si>
     <t>https://www.geeksforgeeks.org/problems/check-if-an-array-is-sorted0701/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article</t>
   </si>
   <si>
@@ -248,6 +245,15 @@
   </si>
   <si>
     <t>https://www.geeksforgeeks.org/problems/second-largest3735/1</t>
+  </si>
+  <si>
+    <t>Check if array is sorted or not</t>
+  </si>
+  <si>
+    <t>Check if a array sorted or not.</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/problems/check-if-an-array-is-sorted0701/1</t>
   </si>
 </sst>
 </file>
@@ -338,7 +344,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -405,15 +411,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -421,6 +418,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -810,8 +819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -825,23 +834,23 @@
   <sheetData>
     <row r="1" spans="1:8" s="12" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="2" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="30" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -856,7 +865,7 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26"/>
+      <c r="A3" s="30"/>
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
@@ -921,12 +930,12 @@
       <c r="D7" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="27" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="30" t="s">
         <v>19</v>
       </c>
       <c r="B8" t="s">
@@ -940,7 +949,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="26"/>
+      <c r="A9" s="30"/>
       <c r="B9" t="s">
         <v>22</v>
       </c>
@@ -1071,45 +1080,46 @@
       <c r="D18" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="29" t="s">
+      <c r="E18" s="26" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="24" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="31" t="s">
-        <v>55</v>
+      <c r="B19" s="28" t="s">
+        <v>54</v>
       </c>
       <c r="C19" s="22"/>
-      <c r="D19" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="29" t="s">
+      <c r="D19" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="26" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="36.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="32"/>
-      <c r="B20" s="31"/>
-      <c r="D20" s="32"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="28"/>
+      <c r="D20" s="29"/>
       <c r="E20" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
+    <row r="21" spans="1:5" s="24" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="20">
         <v>45424</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="22"/>
+      <c r="D21" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="33" t="s">
         <v>52</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.3">
@@ -1117,14 +1127,14 @@
         <v>45425</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C22" s="16"/>
       <c r="D22" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1132,13 +1142,13 @@
         <v>45427</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1146,7 +1156,7 @@
         <v>45568</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C24" s="15"/>
       <c r="D24" s="1" t="s">
@@ -1159,13 +1169,13 @@
         <v>45569</v>
       </c>
       <c r="B25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1173,7 +1183,7 @@
         <v>45588</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>8</v>
@@ -1185,7 +1195,7 @@
         <v>45607</v>
       </c>
       <c r="B27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>8</v>
@@ -1197,13 +1207,13 @@
         <v>45788</v>
       </c>
       <c r="B28" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>69</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1248,7 +1258,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1262,26 +1272,26 @@
   <sheetData>
     <row r="1" spans="1:5" s="12" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="3" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" s="28"/>
+      <c r="C3" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="32"/>
     </row>
     <row r="5" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19">
@@ -1314,7 +1324,7 @@
         <v>8</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -1322,7 +1332,7 @@
         <v>45809</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" s="7">
         <v>1</v>
@@ -1331,10 +1341,28 @@
         <v>8</v>
       </c>
       <c r="E7" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="19">
+        <v>45809</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>73</v>
       </c>
+      <c r="C8" s="7">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B13" s="7"/>
       <c r="C13" s="25"/>
     </row>
   </sheetData>
@@ -1345,8 +1373,9 @@
     <hyperlink ref="E5" r:id="rId1" xr:uid="{C7EF376E-3702-4808-933E-669DEA923A87}"/>
     <hyperlink ref="E6" r:id="rId2" xr:uid="{37D656AF-15C2-4519-B109-B0F60B16F87F}"/>
     <hyperlink ref="E7" r:id="rId3" xr:uid="{C176BE23-95CB-44A1-B207-E06026DD7732}"/>
+    <hyperlink ref="E8" r:id="rId4" xr:uid="{7FEF80E4-D8FA-4309-8AE1-625A51C8CCF2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Remove duplicate in the sorted array
</commit_message>
<xml_diff>
--- a/DSA(2024).xlsx
+++ b/DSA(2024).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaMasterClass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A425628-3198-4DA7-AA9B-E4DBE942A5D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E32F7E-79C9-4B74-B68C-4CC2EEF6FBC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="72">
   <si>
     <t>01-01-2024</t>
   </si>
@@ -166,15 +166,9 @@
     <t>https://www.geeksforgeeks.org/problems/find-the-smallest-and-second-smallest-element-in-an-array3226/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article</t>
   </si>
   <si>
-    <t>https://www.geeksforgeeks.org/problems/remove-duplicate-elements-from-sorted-array/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article</t>
-  </si>
-  <si>
     <t>Find the smallest and second smallest element in an array</t>
   </si>
   <si>
-    <t>Remove Duplicates in-place from Sorted Array</t>
-  </si>
-  <si>
     <t>https://www.geeksforgeeks.org/problems/rotate-array-by-n-elements-1587115621/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article</t>
   </si>
   <si>
@@ -239,6 +233,15 @@
   </si>
   <si>
     <t>=</t>
+  </si>
+  <si>
+    <t>🔁 Level 2: Array Manipulation &amp; Rotations</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Remove Duplicates in-place from Sorted Array</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/problems/remove-duplicate-elements-from-sorted-array/1</t>
   </si>
 </sst>
 </file>
@@ -270,12 +273,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
@@ -296,8 +293,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -322,6 +326,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -336,7 +346,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -357,9 +367,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -379,9 +386,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -392,8 +396,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -405,11 +409,20 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -797,40 +810,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView topLeftCell="C5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="70.5546875" customWidth="1"/>
-    <col min="3" max="3" width="19" style="14" customWidth="1"/>
+    <col min="3" max="3" width="19" style="13" customWidth="1"/>
     <col min="4" max="4" width="18.109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="103.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="12" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:8" s="11" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="2" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -845,7 +858,7 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25"/>
+      <c r="A3" s="23"/>
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
@@ -860,10 +873,10 @@
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="15"/>
+      <c r="C4" s="14"/>
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
@@ -886,7 +899,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="23" t="s">
         <v>17</v>
       </c>
       <c r="B6" t="s">
@@ -900,7 +913,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="25"/>
+      <c r="A7" s="23"/>
       <c r="B7" t="s">
         <v>20</v>
       </c>
@@ -944,7 +957,7 @@
       <c r="B10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="15"/>
+      <c r="C10" s="14"/>
       <c r="D10" s="1" t="s">
         <v>2</v>
       </c>
@@ -1021,96 +1034,81 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="36.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="19"/>
-      <c r="B16" s="20"/>
-      <c r="D16" s="19"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="18"/>
+      <c r="D16" s="17"/>
       <c r="E16" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
-        <v>45425</v>
-      </c>
-      <c r="B17" s="8" t="s">
+        <v>45427</v>
+      </c>
+      <c r="B17" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="16"/>
       <c r="D17" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
-        <v>45427</v>
-      </c>
-      <c r="B18" t="s">
+        <v>45568</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>45569</v>
+      </c>
+      <c r="B19" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
-        <v>45568</v>
-      </c>
-      <c r="B19" s="4" t="s">
+      <c r="D19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
-        <v>45569</v>
+        <v>45607</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>53</v>
-      </c>
+      <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
-        <v>45607</v>
+        <v>45788</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
-        <v>45788</v>
-      </c>
-      <c r="B22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="K22" t="s">
-        <v>70</v>
+      <c r="E21" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="K21" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1132,10 +1130,9 @@
     <hyperlink ref="E13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
     <hyperlink ref="E15" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
     <hyperlink ref="E16" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="E17" r:id="rId14" xr:uid="{60C1110F-5F35-4BA3-BE0E-5D2B2A5A0CB4}"/>
-    <hyperlink ref="E18" r:id="rId15" xr:uid="{CF0FEC0D-8FF8-4FA8-9FED-790E8E16F911}"/>
-    <hyperlink ref="E20" r:id="rId16" xr:uid="{9DAD39F5-2A80-4390-9BA5-B159E91EB2B4}"/>
-    <hyperlink ref="E22" r:id="rId17" xr:uid="{6609612F-5719-43A8-AFA3-447F2B3A4DE5}"/>
+    <hyperlink ref="E17" r:id="rId14" xr:uid="{CF0FEC0D-8FF8-4FA8-9FED-790E8E16F911}"/>
+    <hyperlink ref="E19" r:id="rId15" xr:uid="{9DAD39F5-2A80-4390-9BA5-B159E91EB2B4}"/>
+    <hyperlink ref="E21" r:id="rId16" xr:uid="{6609612F-5719-43A8-AFA3-447F2B3A4DE5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1144,53 +1141,53 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAEC6806-FDB1-4EFE-A78B-6EB62B7514F6}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.88671875" customWidth="1"/>
     <col min="2" max="2" width="13.109375" customWidth="1"/>
-    <col min="3" max="3" width="64.33203125" customWidth="1"/>
-    <col min="4" max="4" width="17.109375" customWidth="1"/>
-    <col min="5" max="5" width="18.77734375" customWidth="1"/>
+    <col min="3" max="3" width="60" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" customWidth="1"/>
+    <col min="5" max="5" width="30.44140625" customWidth="1"/>
     <col min="6" max="6" width="79.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="24" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="13" t="s">
+    <row r="1" spans="1:6" s="22" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="F1" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" s="23" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="3" spans="1:6" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="E3" s="27"/>
+      <c r="D3" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="25"/>
     </row>
     <row r="5" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>1</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="16">
         <v>45809</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1210,7 +1207,7 @@
       <c r="A6" s="7">
         <v>2</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="16">
         <v>45809</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -1223,18 +1220,18 @@
         <v>8</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>3</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="16">
         <v>45809</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D7" s="7">
         <v>1</v>
@@ -1243,18 +1240,18 @@
         <v>8</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>4</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="16">
         <v>45809</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D8" s="7">
         <v>1</v>
@@ -1263,18 +1260,18 @@
         <v>8</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>5</v>
       </c>
-      <c r="B9" s="18">
+      <c r="B9" s="16">
         <v>45811</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D9" s="7">
         <v>1</v>
@@ -1283,14 +1280,14 @@
         <v>8</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>6</v>
       </c>
-      <c r="B10" s="18">
+      <c r="B10" s="16">
         <v>45812</v>
       </c>
       <c r="C10" s="7" t="s">
@@ -1310,11 +1307,11 @@
       <c r="A11" s="7">
         <v>7</v>
       </c>
-      <c r="B11" s="18">
+      <c r="B11" s="16">
         <v>45813</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D11" s="7">
         <v>1</v>
@@ -1323,16 +1320,47 @@
         <v>8</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C13" s="7"/>
-      <c r="D13" s="21"/>
+      <c r="D13" s="19"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D14" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="27"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+    </row>
+    <row r="17" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="7">
+        <v>8</v>
+      </c>
+      <c r="B17" s="16">
+        <v>45814</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="7">
+        <v>1</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="28" t="s">
+        <v>71</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D14:E15"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F5" r:id="rId1" xr:uid="{C7EF376E-3702-4808-933E-669DEA923A87}"/>
@@ -1341,8 +1369,9 @@
     <hyperlink ref="F8" r:id="rId4" xr:uid="{7FEF80E4-D8FA-4309-8AE1-625A51C8CCF2}"/>
     <hyperlink ref="F10" r:id="rId5" xr:uid="{41458DA7-08F1-4101-B7EF-C6C4C1DBA68D}"/>
     <hyperlink ref="F11" r:id="rId6" xr:uid="{0E287AA5-4CDC-47D6-BE0F-CE39ACE52242}"/>
+    <hyperlink ref="F17" r:id="rId7" xr:uid="{6549F3C5-1118-4BDA-9A13-7344D2EC3786}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Left rotate array kth position
</commit_message>
<xml_diff>
--- a/DSA(2024).xlsx
+++ b/DSA(2024).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaMasterClass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E32F7E-79C9-4B74-B68C-4CC2EEF6FBC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B15172-D425-4B29-9A98-E7B71DAD12E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="74">
   <si>
     <t>01-01-2024</t>
   </si>
@@ -242,6 +242,12 @@
   </si>
   <si>
     <t>https://www.geeksforgeeks.org/problems/remove-duplicate-elements-from-sorted-array/1</t>
+  </si>
+  <si>
+    <t>Left Rotate the Array by One and Kth</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/problems/rotate-array-by-n-elements-1587115621/1</t>
   </si>
 </sst>
 </file>
@@ -346,7 +352,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -358,9 +364,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -406,6 +409,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -420,9 +426,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -812,33 +815,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="70.5546875" customWidth="1"/>
-    <col min="3" max="3" width="19" style="13" customWidth="1"/>
+    <col min="3" max="3" width="19" style="12" customWidth="1"/>
     <col min="4" max="4" width="18.109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="103.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="11" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:8" s="10" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>57</v>
       </c>
     </row>
@@ -846,7 +849,7 @@
       <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -859,7 +862,7 @@
     </row>
     <row r="3" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="23"/>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -873,10 +876,10 @@
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="14"/>
+      <c r="C4" s="13"/>
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
@@ -888,7 +891,7 @@
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -957,7 +960,7 @@
       <c r="B10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="14"/>
+      <c r="C10" s="13"/>
       <c r="D10" s="1" t="s">
         <v>2</v>
       </c>
@@ -1034,9 +1037,9 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="36.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
-      <c r="B16" s="18"/>
-      <c r="D16" s="17"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="17"/>
+      <c r="D16" s="16"/>
       <c r="E16" s="4" t="s">
         <v>45</v>
       </c>
@@ -1062,7 +1065,7 @@
       <c r="B18" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="14"/>
+      <c r="C18" s="13"/>
       <c r="D18" s="1" t="s">
         <v>8</v>
       </c>
@@ -1078,7 +1081,7 @@
       <c r="D19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="5" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1104,7 +1107,7 @@
       <c r="D21" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="5" t="s">
         <v>60</v>
       </c>
       <c r="K21" t="s">
@@ -1141,10 +1144,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAEC6806-FDB1-4EFE-A78B-6EB62B7514F6}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1157,23 +1160,23 @@
     <col min="6" max="6" width="79.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="22" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:6" s="21" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="20" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1183,149 +1186,149 @@
       </c>
       <c r="E3" s="25"/>
     </row>
-    <row r="5" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7">
+    <row r="5" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
         <v>1</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="15">
         <v>45809</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>1</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="6" t="s">
+      <c r="E5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7">
+    <row r="6" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
         <v>2</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="15">
         <v>45809</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="6">
         <v>1</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="6" t="s">
+      <c r="E6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7">
+    <row r="7" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
         <v>3</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7" s="15">
         <v>45809</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>1</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="6" t="s">
+      <c r="E7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7">
+    <row r="8" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
         <v>4</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="15">
         <v>45809</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="6">
         <v>1</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="6" t="s">
+      <c r="E8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7">
+    <row r="9" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
         <v>5</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="15">
         <v>45811</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <v>1</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="7" t="s">
+      <c r="E9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7">
+    <row r="10" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
         <v>6</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="15">
         <v>45812</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="6">
         <v>1</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="6" t="s">
+      <c r="E10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7">
+    <row r="11" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
         <v>7</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="15">
         <v>45813</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="6">
         <v>1</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="6" t="s">
+      <c r="E11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C13" s="7"/>
-      <c r="D13" s="19"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="18"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D14" s="26" t="s">
@@ -1337,24 +1340,44 @@
       <c r="D15" s="27"/>
       <c r="E15" s="27"/>
     </row>
-    <row r="17" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="7">
-        <v>8</v>
-      </c>
-      <c r="B17" s="16">
+    <row r="17" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="6">
+        <v>8</v>
+      </c>
+      <c r="B17" s="15">
         <v>45814</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="6">
         <v>1</v>
       </c>
-      <c r="E17" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="28" t="s">
+      <c r="E17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="22" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="6">
+        <v>9</v>
+      </c>
+      <c r="B18" s="15">
+        <v>45815</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="6">
+        <v>1</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1370,8 +1393,9 @@
     <hyperlink ref="F10" r:id="rId5" xr:uid="{41458DA7-08F1-4101-B7EF-C6C4C1DBA68D}"/>
     <hyperlink ref="F11" r:id="rId6" xr:uid="{0E287AA5-4CDC-47D6-BE0F-CE39ACE52242}"/>
     <hyperlink ref="F17" r:id="rId7" xr:uid="{6549F3C5-1118-4BDA-9A13-7344D2EC3786}"/>
+    <hyperlink ref="F18" r:id="rId8" xr:uid="{7AC10858-094E-41DF-981F-826370220531}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Matrix, Ceiling and floor of a number
</commit_message>
<xml_diff>
--- a/DSA(2024).xlsx
+++ b/DSA(2024).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaMasterClass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A7750E-46A5-46DD-8134-42AE2E4D93A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A2DDD5B-CB05-4A44-BDCB-20D385D992CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="72">
   <si>
     <t>01-01-2024</t>
   </si>
@@ -79,9 +79,6 @@
     <t>https://leetcode.com/problems/length-of-last-word/description/</t>
   </si>
   <si>
-    <t>08-01-2024</t>
-  </si>
-  <si>
     <t>Ceiling of a Number</t>
   </si>
   <si>
@@ -136,18 +133,9 @@
     <t>https://leetcode.com/problems/search-in-rotated-sorted-array-ii/description/</t>
   </si>
   <si>
-    <t>15-01-2024</t>
-  </si>
-  <si>
-    <t>Rotation Count</t>
-  </si>
-  <si>
     <t>https://www.geeksforgeeks.org/find-rotation-count-rotated-sorted-array/</t>
   </si>
   <si>
-    <t>17-01-2024</t>
-  </si>
-  <si>
     <t>Row Column Matrix</t>
   </si>
   <si>
@@ -251,13 +239,16 @@
   </si>
   <si>
     <t>Rotation count</t>
+  </si>
+  <si>
+    <t>🔍 Level 3: Search &amp; Binary Search Variants</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -309,6 +300,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -355,7 +352,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -415,15 +412,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -437,6 +425,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -825,10 +819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -842,23 +836,23 @@
   <sheetData>
     <row r="1" spans="1:8" s="10" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>58</v>
-      </c>
       <c r="D1" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -873,7 +867,7 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26"/>
+      <c r="A3" s="23"/>
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
@@ -913,242 +907,198 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
-        <v>17</v>
-      </c>
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26"/>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E7" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="13"/>
       <c r="D9" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="13"/>
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
       <c r="D10" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="17" customFormat="1" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>39</v>
       </c>
+    </row>
+    <row r="13" spans="1:8" ht="36.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="16"/>
+      <c r="B13" s="17"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>45427</v>
+      </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" t="s">
-        <v>42</v>
-      </c>
+      <c r="E14" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>45568</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="13"/>
       <c r="D15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="36.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="16"/>
-      <c r="B16" s="17"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>45569</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
-        <v>45427</v>
+        <v>45607</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
-        <v>45568</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="13"/>
+        <v>45788</v>
+      </c>
+      <c r="B18" t="s">
+        <v>55</v>
+      </c>
       <c r="D18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
-        <v>45569</v>
-      </c>
-      <c r="B19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
-        <v>45607</v>
-      </c>
-      <c r="B20" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
-        <v>45788</v>
-      </c>
-      <c r="B21" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="K21" t="s">
-        <v>68</v>
+      <c r="E18" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="K18" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A6:A7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="E5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="E6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="E9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="E10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="E12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="E13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="E15" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="E16" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="E17" r:id="rId14" xr:uid="{CF0FEC0D-8FF8-4FA8-9FED-790E8E16F911}"/>
-    <hyperlink ref="E19" r:id="rId15" xr:uid="{9DAD39F5-2A80-4390-9BA5-B159E91EB2B4}"/>
-    <hyperlink ref="E21" r:id="rId16" xr:uid="{6609612F-5719-43A8-AFA3-447F2B3A4DE5}"/>
+    <hyperlink ref="E7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="E12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="E13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="E14" r:id="rId12" xr:uid="{CF0FEC0D-8FF8-4FA8-9FED-790E8E16F911}"/>
+    <hyperlink ref="E16" r:id="rId13" xr:uid="{9DAD39F5-2A80-4390-9BA5-B159E91EB2B4}"/>
+    <hyperlink ref="E18" r:id="rId14" xr:uid="{6609612F-5719-43A8-AFA3-447F2B3A4DE5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1157,10 +1107,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAEC6806-FDB1-4EFE-A78B-6EB62B7514F6}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1170,34 +1120,34 @@
     <col min="3" max="3" width="60" customWidth="1"/>
     <col min="4" max="4" width="18.88671875" customWidth="1"/>
     <col min="5" max="5" width="30.44140625" customWidth="1"/>
-    <col min="6" max="6" width="79.21875" customWidth="1"/>
+    <col min="6" max="6" width="89.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="21" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>58</v>
-      </c>
       <c r="E1" s="11" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F1" s="20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="24" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="E3" s="28"/>
+      <c r="E3" s="25"/>
     </row>
     <row r="5" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
@@ -1227,7 +1177,7 @@
         <v>45809</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D6" s="6">
         <v>1</v>
@@ -1236,7 +1186,7 @@
         <v>8</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -1247,7 +1197,7 @@
         <v>45809</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D7" s="6">
         <v>1</v>
@@ -1256,7 +1206,7 @@
         <v>8</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -1267,7 +1217,7 @@
         <v>45809</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D8" s="6">
         <v>1</v>
@@ -1276,7 +1226,7 @@
         <v>8</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -1287,7 +1237,7 @@
         <v>45811</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D9" s="6">
         <v>1</v>
@@ -1296,7 +1246,7 @@
         <v>8</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -1327,7 +1277,7 @@
         <v>45813</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D11" s="6">
         <v>1</v>
@@ -1336,7 +1286,7 @@
         <v>8</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1344,14 +1294,14 @@
       <c r="D13" s="18"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D14" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="E14" s="30"/>
+      <c r="D14" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="27"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
     </row>
     <row r="17" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
@@ -1361,7 +1311,7 @@
         <v>45814</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D17" s="6">
         <v>1</v>
@@ -1370,7 +1320,7 @@
         <v>8</v>
       </c>
       <c r="F17" s="22" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -1381,7 +1331,7 @@
         <v>45815</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D18" s="6">
         <v>1</v>
@@ -1390,7 +1340,7 @@
         <v>8</v>
       </c>
       <c r="F18" s="22" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -1401,7 +1351,7 @@
         <v>45816</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D19" s="6">
         <v>1</v>
@@ -1410,13 +1360,78 @@
         <v>8</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D23" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" s="29"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+    </row>
+    <row r="26" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="6">
+        <v>11</v>
+      </c>
+      <c r="B26" s="15">
+        <v>45817</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" s="6">
+        <v>1</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="6">
+        <v>12</v>
+      </c>
+      <c r="B27" s="15">
+        <v>45818</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="6">
+        <v>1</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="6">
+        <v>13</v>
+      </c>
+      <c r="B28" s="15">
+        <v>45818</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="6">
+        <v>1</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D14:E15"/>
+    <mergeCell ref="D23:E24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F5" r:id="rId1" xr:uid="{C7EF376E-3702-4808-933E-669DEA923A87}"/>
@@ -1428,8 +1443,9 @@
     <hyperlink ref="F17" r:id="rId7" xr:uid="{6549F3C5-1118-4BDA-9A13-7344D2EC3786}"/>
     <hyperlink ref="F18" r:id="rId8" xr:uid="{7AC10858-094E-41DF-981F-826370220531}"/>
     <hyperlink ref="F19" r:id="rId9" xr:uid="{0F1201B2-948D-4121-80DE-40118D381BDB}"/>
+    <hyperlink ref="F27" r:id="rId10" xr:uid="{7B91D10A-40CC-4E2E-B48C-C36796C65A28}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Smallest and second smallest
</commit_message>
<xml_diff>
--- a/DSA(2024).xlsx
+++ b/DSA(2024).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaMasterClass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A2DDD5B-CB05-4A44-BDCB-20D385D992CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE903BB-8870-4CCA-924A-208AE500CBD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="74">
   <si>
     <t>01-01-2024</t>
   </si>
@@ -242,6 +242,12 @@
   </si>
   <si>
     <t>🔍 Level 3: Search &amp; Binary Search Variants</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/to-find-smallest-and-second-smallest-element-in-an-array/</t>
+  </si>
+  <si>
+    <t>Find the second larges element in an array</t>
   </si>
 </sst>
 </file>
@@ -821,7 +827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
@@ -1109,8 +1115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAEC6806-FDB1-4EFE-A78B-6EB62B7514F6}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1197,7 +1203,7 @@
         <v>45809</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="D7" s="6">
         <v>1</v>
@@ -1287,6 +1293,26 @@
       </c>
       <c r="F11" s="5" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6">
+        <v>8</v>
+      </c>
+      <c r="B12" s="15">
+        <v>45818</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="6">
+        <v>1</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1444,8 +1470,9 @@
     <hyperlink ref="F18" r:id="rId8" xr:uid="{7AC10858-094E-41DF-981F-826370220531}"/>
     <hyperlink ref="F19" r:id="rId9" xr:uid="{0F1201B2-948D-4121-80DE-40118D381BDB}"/>
     <hyperlink ref="F27" r:id="rId10" xr:uid="{7B91D10A-40CC-4E2E-B48C-C36796C65A28}"/>
+    <hyperlink ref="F12" r:id="rId11" xr:uid="{9B4A9039-AEC6-4ECB-978F-74F971987074}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Find first and last in sorted array
</commit_message>
<xml_diff>
--- a/DSA(2024).xlsx
+++ b/DSA(2024).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaMasterClass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF758452-43CC-4497-9424-B8D89A7264F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE32859-BD52-4394-9C6C-9A201E98222B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="74">
   <si>
     <t>01-01-2024</t>
   </si>
@@ -358,7 +358,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -418,6 +418,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -439,7 +440,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -829,7 +835,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -859,7 +865,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -874,7 +880,7 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="23"/>
+      <c r="A3" s="24"/>
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
@@ -924,21 +930,22 @@
       <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:8" s="17" customFormat="1" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="C7" s="32"/>
+      <c r="D7" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="23" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1104,10 +1111,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAEC6806-FDB1-4EFE-A78B-6EB62B7514F6}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1141,10 +1148,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="25"/>
+      <c r="E3" s="26"/>
     </row>
     <row r="5" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
@@ -1311,14 +1318,14 @@
       <c r="D13" s="18"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D14" s="26" t="s">
+      <c r="D14" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="E14" s="27"/>
+      <c r="E14" s="28"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
     </row>
     <row r="17" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
@@ -1381,14 +1388,14 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D23" s="28" t="s">
+      <c r="D23" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="E23" s="29"/>
+      <c r="E23" s="30"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
     </row>
     <row r="26" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
@@ -1462,6 +1469,26 @@
       </c>
       <c r="F29" s="22" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="6">
+        <v>16</v>
+      </c>
+      <c r="B30" s="15">
+        <v>45823</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" s="6">
+        <v>1</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F30" s="22" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1483,8 +1510,9 @@
     <hyperlink ref="F27" r:id="rId10" xr:uid="{7B91D10A-40CC-4E2E-B48C-C36796C65A28}"/>
     <hyperlink ref="F12" r:id="rId11" xr:uid="{9B4A9039-AEC6-4ECB-978F-74F971987074}"/>
     <hyperlink ref="F29" r:id="rId12" xr:uid="{1FA02A46-3A34-4B69-9C03-08E941DA5C48}"/>
+    <hyperlink ref="F30" r:id="rId13" xr:uid="{F4A19F1B-5F7C-4A5D-84C7-734209434470}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Find position element in sorted array
</commit_message>
<xml_diff>
--- a/DSA(2024).xlsx
+++ b/DSA(2024).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaMasterClass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE32859-BD52-4394-9C6C-9A201E98222B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C318EDF7-3558-439A-AB2F-62D1AA069CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="72">
   <si>
     <t>01-01-2024</t>
   </si>
@@ -46,9 +46,6 @@
     <t>https://leetcode.com/problems/3sum/description/</t>
   </si>
   <si>
-    <t>02-01-2024</t>
-  </si>
-  <si>
     <t>Position of an Element in Infinite Sorted Array</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/find-smallest-letter-greater-than-target/</t>
-  </si>
-  <si>
-    <t>10-01-2024</t>
   </si>
   <si>
     <t>First and Last Position in Sorted Array</t>
@@ -358,7 +352,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -375,9 +369,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -438,12 +429,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -832,40 +817,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="70.5546875" customWidth="1"/>
-    <col min="3" max="3" width="19" style="12" customWidth="1"/>
+    <col min="3" max="3" width="19" style="11" customWidth="1"/>
     <col min="4" max="4" width="18.109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="103.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="10" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:11" s="9" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+    </row>
+    <row r="2" spans="1:11" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -879,8 +864,8 @@
       </c>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="24"/>
+    <row r="3" spans="1:11" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="23"/>
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
@@ -891,197 +876,167 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="13"/>
+        <v>9</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>11</v>
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="12"/>
       <c r="D6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="17" customFormat="1" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="13"/>
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
       <c r="D8" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>37</v>
       </c>
+    </row>
+    <row r="10" spans="1:11" ht="36.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="15"/>
+      <c r="B10" s="16"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>45427</v>
+      </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="36.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="16"/>
-      <c r="B12" s="17"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>45568</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
-        <v>45427</v>
+        <v>45569</v>
       </c>
       <c r="B13" t="s">
         <v>44</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
-        <v>45568</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="13"/>
+        <v>45607</v>
+      </c>
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
       <c r="D14" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
-        <v>45569</v>
+        <v>45788</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
-        <v>45607</v>
-      </c>
-      <c r="B16" t="s">
-        <v>49</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
-        <v>45788</v>
-      </c>
-      <c r="B17" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="K17" t="s">
-        <v>64</v>
+        <v>54</v>
+      </c>
+      <c r="K15" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1091,18 +1046,16 @@
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="E6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="E7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="E8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="E10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="E11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="E12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="E13" r:id="rId12" xr:uid="{CF0FEC0D-8FF8-4FA8-9FED-790E8E16F911}"/>
-    <hyperlink ref="E15" r:id="rId13" xr:uid="{9DAD39F5-2A80-4390-9BA5-B159E91EB2B4}"/>
-    <hyperlink ref="E17" r:id="rId14" xr:uid="{6609612F-5719-43A8-AFA3-447F2B3A4DE5}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="E10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="E11" r:id="rId10" xr:uid="{CF0FEC0D-8FF8-4FA8-9FED-790E8E16F911}"/>
+    <hyperlink ref="E13" r:id="rId11" xr:uid="{9DAD39F5-2A80-4390-9BA5-B159E91EB2B4}"/>
+    <hyperlink ref="E15" r:id="rId12" xr:uid="{6609612F-5719-43A8-AFA3-447F2B3A4DE5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1111,10 +1064,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAEC6806-FDB1-4EFE-A78B-6EB62B7514F6}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1127,368 +1080,388 @@
     <col min="6" max="6" width="89.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="21" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="1:6" s="20" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="F1" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="3" spans="1:6" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="26"/>
+      <c r="D3" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="25"/>
     </row>
     <row r="5" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>1</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="14">
         <v>45809</v>
       </c>
       <c r="C5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="D5" s="6">
-        <v>1</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>2</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>45809</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D6" s="6">
         <v>1</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>3</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="14">
         <v>45809</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D7" s="6">
         <v>1</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>4</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="14">
         <v>45809</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D8" s="6">
         <v>1</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>5</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="14">
         <v>45811</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D9" s="6">
         <v>1</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>6</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="14">
         <v>45812</v>
       </c>
       <c r="C10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="6">
+        <v>1</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="D10" s="6">
-        <v>1</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>7</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="14">
         <v>45813</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D11" s="6">
         <v>1</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>8</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="14">
         <v>45818</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D12" s="6">
         <v>1</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C13" s="6"/>
-      <c r="D13" s="18"/>
+      <c r="D13" s="17"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D14" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="E14" s="28"/>
+      <c r="D14" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="27"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
     </row>
     <row r="17" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>9</v>
       </c>
-      <c r="B17" s="15">
+      <c r="B17" s="14">
         <v>45814</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D17" s="6">
         <v>1</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="22" t="s">
-        <v>67</v>
+        <v>7</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>10</v>
       </c>
-      <c r="B18" s="15">
+      <c r="B18" s="14">
         <v>45815</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D18" s="6">
         <v>1</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="22" t="s">
-        <v>69</v>
+        <v>7</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>11</v>
       </c>
-      <c r="B19" s="15">
+      <c r="B19" s="14">
         <v>45816</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D19" s="6">
         <v>1</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D23" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="E23" s="30"/>
+      <c r="D23" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E23" s="29"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
     </row>
     <row r="26" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>12</v>
       </c>
-      <c r="B26" s="15">
+      <c r="B26" s="14">
         <v>45817</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D26" s="6">
         <v>1</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>13</v>
       </c>
-      <c r="B27" s="15">
+      <c r="B27" s="14">
         <v>45818</v>
       </c>
       <c r="C27" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="6">
+        <v>1</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="21" t="s">
         <v>17</v>
-      </c>
-      <c r="D27" s="6">
-        <v>1</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F27" s="22" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>14</v>
       </c>
-      <c r="B28" s="15">
+      <c r="B28" s="14">
         <v>45818</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D28" s="6">
         <v>1</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>15</v>
       </c>
-      <c r="B29" s="15">
+      <c r="B29" s="14">
         <v>45819</v>
       </c>
       <c r="C29" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" s="6">
+        <v>1</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="21" t="s">
         <v>21</v>
-      </c>
-      <c r="D29" s="6">
-        <v>1</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F29" s="22" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>16</v>
       </c>
-      <c r="B30" s="15">
+      <c r="B30" s="14">
         <v>45823</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D30" s="6">
         <v>1</v>
       </c>
       <c r="E30" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="6">
+        <v>17</v>
+      </c>
+      <c r="B31" s="14">
+        <v>45824</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="6">
+        <v>1</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="F30" s="22" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1511,8 +1484,9 @@
     <hyperlink ref="F12" r:id="rId11" xr:uid="{9B4A9039-AEC6-4ECB-978F-74F971987074}"/>
     <hyperlink ref="F29" r:id="rId12" xr:uid="{1FA02A46-3A34-4B69-9C03-08E941DA5C48}"/>
     <hyperlink ref="F30" r:id="rId13" xr:uid="{F4A19F1B-5F7C-4A5D-84C7-734209434470}"/>
+    <hyperlink ref="F31" r:id="rId14" xr:uid="{B66EF7D4-A824-4EC8-8F39-AB907090ED11}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added some code and changes
</commit_message>
<xml_diff>
--- a/DSA(2024).xlsx
+++ b/DSA(2024).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaMasterClass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C318EDF7-3558-439A-AB2F-62D1AA069CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EDDEA9C-13C5-4866-8B49-3B401160FD5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="93">
   <si>
     <t>01-01-2024</t>
   </si>
@@ -220,9 +220,6 @@
     <t>🔁 Level 2: Array Manipulation &amp; Rotations</t>
   </si>
   <si>
-    <t xml:space="preserve"> Remove Duplicates in-place from Sorted Array</t>
-  </si>
-  <si>
     <t>https://www.geeksforgeeks.org/problems/remove-duplicate-elements-from-sorted-array/1</t>
   </si>
   <si>
@@ -242,6 +239,72 @@
   </si>
   <si>
     <t>Find the second larges element in an array</t>
+  </si>
+  <si>
+    <t>INTERVIEW</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>CLASS NAME</t>
+  </si>
+  <si>
+    <t>ValidAnagram</t>
+  </si>
+  <si>
+    <t>SecondLargest</t>
+  </si>
+  <si>
+    <t>Remove Duplicates in-place from Sorted Array</t>
+  </si>
+  <si>
+    <t>FindPositionElement</t>
+  </si>
+  <si>
+    <t>FindFirstAndLast</t>
+  </si>
+  <si>
+    <t>Ceiling</t>
+  </si>
+  <si>
+    <t>Floor</t>
+  </si>
+  <si>
+    <t>SmallestLetter</t>
+  </si>
+  <si>
+    <t>RowColMatrix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SearchRotatedSortedArray </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Search in Rotated Sorted Array</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>⛰️ Level 4: Bit  Challenging Search &amp; Peak Logic</t>
+  </si>
+  <si>
+    <t>http://leetcode.com/problems/peak-index-in-a-mountain-array/description/</t>
+  </si>
+  <si>
+    <t>PeakIndexInMountainArr</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Find in Mountain Array</t>
+  </si>
+  <si>
+    <t>Hard</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/find-in-mountain-array/submissions/1848951745/</t>
+  </si>
+  <si>
+    <t>FindInMountain</t>
   </si>
 </sst>
 </file>
@@ -1064,23 +1127,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAEC6806-FDB1-4EFE-A78B-6EB62B7514F6}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.88671875" customWidth="1"/>
     <col min="2" max="2" width="13.109375" customWidth="1"/>
-    <col min="3" max="3" width="60" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" customWidth="1"/>
-    <col min="5" max="5" width="30.44140625" customWidth="1"/>
-    <col min="6" max="6" width="89.77734375" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" customWidth="1"/>
+    <col min="5" max="5" width="60" customWidth="1"/>
+    <col min="6" max="6" width="18.88671875" customWidth="1"/>
+    <col min="7" max="7" width="32.33203125" customWidth="1"/>
+    <col min="8" max="8" width="89.77734375" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="20" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="20" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>61</v>
       </c>
@@ -1088,405 +1154,542 @@
         <v>48</v>
       </c>
       <c r="C1" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="H1" s="19" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="24" t="s">
+      <c r="I1" s="18"/>
+    </row>
+    <row r="3" spans="1:9" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="25"/>
-    </row>
-    <row r="5" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="25"/>
+    </row>
+    <row r="5" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>1</v>
       </c>
       <c r="B5" s="14">
         <v>45809</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="6">
-        <v>1</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="6">
+        <v>1</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>2</v>
       </c>
       <c r="B6" s="14">
         <v>45809</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="6">
-        <v>1</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>3</v>
       </c>
       <c r="B7" s="14">
         <v>45809</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D7" s="6">
-        <v>1</v>
+      <c r="C7" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>72</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="6">
+        <v>1</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>4</v>
       </c>
       <c r="B8" s="14">
         <v>45809</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D8" s="6">
-        <v>1</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="6">
+        <v>1</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>5</v>
       </c>
       <c r="B9" s="14">
         <v>45811</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="6">
-        <v>1</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="6">
+        <v>1</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>6</v>
       </c>
       <c r="B10" s="14">
         <v>45812</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="6">
-        <v>1</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="6">
+        <v>1</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>7</v>
       </c>
       <c r="B11" s="14">
         <v>45813</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="6">
-        <v>1</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="6">
+        <v>1</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>8</v>
       </c>
       <c r="B12" s="14">
         <v>45818</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="6">
-        <v>1</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C13" s="6"/>
-      <c r="D13" s="17"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D14" s="26" t="s">
+      <c r="F12" s="6">
+        <v>1</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E13" s="6"/>
+      <c r="F13" s="17"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F14" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="27"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-    </row>
-    <row r="17" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G14" s="27"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+    </row>
+    <row r="17" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>9</v>
       </c>
       <c r="B17" s="14">
         <v>45814</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" s="6">
+        <v>1</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H17" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="D17" s="6">
-        <v>1</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" s="21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>10</v>
       </c>
       <c r="B18" s="14">
         <v>45815</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="6">
+        <v>1</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D18" s="6">
-        <v>1</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" s="21" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>11</v>
       </c>
       <c r="B19" s="14">
         <v>45816</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" s="6">
+        <v>1</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F23" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="D19" s="6">
-        <v>1</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D23" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="E23" s="29"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-    </row>
-    <row r="26" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G23" s="29"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+    </row>
+    <row r="26" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>12</v>
       </c>
       <c r="B26" s="14">
         <v>45817</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" s="14"/>
+      <c r="E26" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="6">
-        <v>1</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F26" s="6">
+        <v>1</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>13</v>
       </c>
       <c r="B27" s="14">
         <v>45818</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27" s="14"/>
+      <c r="E27" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D27" s="6">
-        <v>1</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F27" s="21" t="s">
+      <c r="F27" s="6">
+        <v>1</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" s="21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>14</v>
       </c>
       <c r="B28" s="14">
         <v>45818</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D28" s="14"/>
+      <c r="E28" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="6">
-        <v>1</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F28" s="6">
+        <v>1</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>15</v>
       </c>
       <c r="B29" s="14">
         <v>45819</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" s="14"/>
+      <c r="E29" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D29" s="6">
-        <v>1</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F29" s="21" t="s">
+      <c r="F29" s="6">
+        <v>1</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29" s="21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>16</v>
       </c>
       <c r="B30" s="14">
         <v>45823</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" s="14"/>
+      <c r="E30" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="6">
-        <v>1</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F30" s="21" t="s">
+      <c r="F30" s="6">
+        <v>1</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H30" s="21" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>17</v>
       </c>
       <c r="B31" s="14">
         <v>45824</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" s="14"/>
+      <c r="E31" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="6">
-        <v>1</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F31" s="5" t="s">
+      <c r="F31" s="6">
+        <v>1</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31" s="5" t="s">
         <v>8</v>
       </c>
     </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="6">
+        <v>18</v>
+      </c>
+      <c r="B32" s="14">
+        <v>45997</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F34" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="G34" s="29"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F35" s="29"/>
+      <c r="G35" s="29"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="6">
+        <v>19</v>
+      </c>
+      <c r="B37" s="14">
+        <v>45997</v>
+      </c>
+      <c r="C37" t="s">
+        <v>88</v>
+      </c>
+      <c r="E37" t="s">
+        <v>10</v>
+      </c>
+      <c r="G37" t="s">
+        <v>85</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="6">
+        <v>20</v>
+      </c>
+      <c r="B38" s="14">
+        <v>45997</v>
+      </c>
+      <c r="C38" t="s">
+        <v>92</v>
+      </c>
+      <c r="E38" t="s">
+        <v>89</v>
+      </c>
+      <c r="G38" t="s">
+        <v>90</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D14:E15"/>
-    <mergeCell ref="D23:E24"/>
+  <mergeCells count="4">
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F14:G15"/>
+    <mergeCell ref="F23:G24"/>
+    <mergeCell ref="F34:G35"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F5" r:id="rId1" xr:uid="{C7EF376E-3702-4808-933E-669DEA923A87}"/>
-    <hyperlink ref="F6" r:id="rId2" xr:uid="{37D656AF-15C2-4519-B109-B0F60B16F87F}"/>
-    <hyperlink ref="F7" r:id="rId3" xr:uid="{C176BE23-95CB-44A1-B207-E06026DD7732}"/>
-    <hyperlink ref="F8" r:id="rId4" xr:uid="{7FEF80E4-D8FA-4309-8AE1-625A51C8CCF2}"/>
-    <hyperlink ref="F10" r:id="rId5" xr:uid="{41458DA7-08F1-4101-B7EF-C6C4C1DBA68D}"/>
-    <hyperlink ref="F11" r:id="rId6" xr:uid="{0E287AA5-4CDC-47D6-BE0F-CE39ACE52242}"/>
-    <hyperlink ref="F17" r:id="rId7" xr:uid="{6549F3C5-1118-4BDA-9A13-7344D2EC3786}"/>
-    <hyperlink ref="F18" r:id="rId8" xr:uid="{7AC10858-094E-41DF-981F-826370220531}"/>
-    <hyperlink ref="F19" r:id="rId9" xr:uid="{0F1201B2-948D-4121-80DE-40118D381BDB}"/>
-    <hyperlink ref="F27" r:id="rId10" xr:uid="{7B91D10A-40CC-4E2E-B48C-C36796C65A28}"/>
-    <hyperlink ref="F12" r:id="rId11" xr:uid="{9B4A9039-AEC6-4ECB-978F-74F971987074}"/>
-    <hyperlink ref="F29" r:id="rId12" xr:uid="{1FA02A46-3A34-4B69-9C03-08E941DA5C48}"/>
-    <hyperlink ref="F30" r:id="rId13" xr:uid="{F4A19F1B-5F7C-4A5D-84C7-734209434470}"/>
-    <hyperlink ref="F31" r:id="rId14" xr:uid="{B66EF7D4-A824-4EC8-8F39-AB907090ED11}"/>
+    <hyperlink ref="H5" r:id="rId1" xr:uid="{C7EF376E-3702-4808-933E-669DEA923A87}"/>
+    <hyperlink ref="H6" r:id="rId2" xr:uid="{37D656AF-15C2-4519-B109-B0F60B16F87F}"/>
+    <hyperlink ref="H7" r:id="rId3" xr:uid="{C176BE23-95CB-44A1-B207-E06026DD7732}"/>
+    <hyperlink ref="H8" r:id="rId4" xr:uid="{7FEF80E4-D8FA-4309-8AE1-625A51C8CCF2}"/>
+    <hyperlink ref="H10" r:id="rId5" xr:uid="{41458DA7-08F1-4101-B7EF-C6C4C1DBA68D}"/>
+    <hyperlink ref="H11" r:id="rId6" xr:uid="{0E287AA5-4CDC-47D6-BE0F-CE39ACE52242}"/>
+    <hyperlink ref="H17" r:id="rId7" xr:uid="{6549F3C5-1118-4BDA-9A13-7344D2EC3786}"/>
+    <hyperlink ref="H18" r:id="rId8" xr:uid="{7AC10858-094E-41DF-981F-826370220531}"/>
+    <hyperlink ref="H19" r:id="rId9" xr:uid="{0F1201B2-948D-4121-80DE-40118D381BDB}"/>
+    <hyperlink ref="H27" r:id="rId10" xr:uid="{7B91D10A-40CC-4E2E-B48C-C36796C65A28}"/>
+    <hyperlink ref="H12" r:id="rId11" xr:uid="{9B4A9039-AEC6-4ECB-978F-74F971987074}"/>
+    <hyperlink ref="H29" r:id="rId12" xr:uid="{1FA02A46-3A34-4B69-9C03-08E941DA5C48}"/>
+    <hyperlink ref="H30" r:id="rId13" xr:uid="{F4A19F1B-5F7C-4A5D-84C7-734209434470}"/>
+    <hyperlink ref="H31" r:id="rId14" xr:uid="{B66EF7D4-A824-4EC8-8F39-AB907090ED11}"/>
+    <hyperlink ref="H32" r:id="rId15" xr:uid="{805C80E5-56F7-4B13-999B-A858CE456807}"/>
+    <hyperlink ref="H37" r:id="rId16" xr:uid="{29D24E6E-7C58-4D8F-B890-61ABB062018A}"/>
+    <hyperlink ref="H38" r:id="rId17" xr:uid="{D5D45557-F426-4724-AEDE-9C4D17575396}"/>
+    <hyperlink ref="H9" r:id="rId18" xr:uid="{8EEBD4CD-CE8C-422A-AE7F-B1EC8E5BF854}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>